<commit_message>
docs(qa): update test case and add test summary report
</commit_message>
<xml_diff>
--- a/qa-docs/test-cases/test-case-document.xlsx
+++ b/qa-docs/test-cases/test-case-document.xlsx
@@ -5,27 +5,39 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanjeewa\Desktop\wire apps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sanjeewa\Desktop\wire apps\New folder\documents\Technical-Assessment-Champika\qa-docs\test-cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2504BBC-0807-48CC-A948-28EB72CB5EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F045912-14DF-49AF-A251-0B60C1BBC1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$46</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="132">
   <si>
     <t>Test case ID</t>
   </si>
@@ -678,6 +690,17 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>Verify whether user can open google translate page in different browsers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the web browser
+2.  Type "https://translate.google.com/?sl=en&amp;tl=si&amp;text=dog%20comming&amp;op=translate" URL in search bar
+</t>
+  </si>
+  <si>
+    <t>User should be able to  open google translate page in different browsers</t>
   </si>
 </sst>
 </file>
@@ -742,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -750,7 +773,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1033,11 +1059,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G11" sqref="G11:G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,875 +1102,953 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="115.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="G2" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="115.8" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="G3" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="G4" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="C5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="G5" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="G6" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="G7" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="C8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="G8" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="C9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="G9" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="C11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+    <row r="12" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="C12" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="G12" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+    <row r="15" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="C15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="G15" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="C16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="C17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+    <row r="18" spans="1:7" ht="201.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="C18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="G18" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="201.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="C19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="G19" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="C20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="G20" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="230.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="C21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="230.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="G21" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="230.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="3" t="s">
+      <c r="C22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
+      <c r="G22" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="C23" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2">
+      <c r="G23" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="C24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="2">
+      <c r="G24" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="C25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2">
+      <c r="G25" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="3" t="s">
+      <c r="C26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2">
+      <c r="G26" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="C27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2">
+      <c r="G27" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="158.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="C28" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A29" s="2">
+      <c r="G28" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="144" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="C29" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="G29" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A30" s="2">
+      <c r="A30" s="3">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="C30" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A31" s="2">
+    <row r="31" spans="1:7" ht="144" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="C31" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A32" s="2">
+      <c r="G31" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="144" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="C32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A33" s="2">
+      <c r="G32" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="144" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
         <v>32</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="3" t="s">
+      <c r="C33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="G33" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A34" s="2">
+      <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="C34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="G34" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A35" s="2">
+      <c r="A35" s="3">
         <v>34</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="C35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="3" t="s">
         <v>81</v>
       </c>
+      <c r="G35" s="3" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="36" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A36" s="2">
+      <c r="A36" s="3">
         <v>35</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="C36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A37" s="2">
+      <c r="A37" s="3">
         <v>36</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="C37" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="G37" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A38" s="2">
+    <row r="38" spans="1:7" ht="144" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
         <v>37</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="3" t="s">
+      <c r="C38" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A39" s="2">
+      <c r="G38" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="144" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="3" t="s">
+      <c r="C39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D39" s="3"/>
+      <c r="E39" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G39" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A40" s="2">
+      <c r="G39" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="144" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
         <v>39</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="3" t="s">
+      <c r="C40" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="3"/>
+      <c r="E40" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="144" x14ac:dyDescent="0.3">
-      <c r="A41" s="2">
+      <c r="G40" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="144" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="C41" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G41" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="2">
+      <c r="G41" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
         <v>41</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="C42" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="G42" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A43" s="2">
+      <c r="G42" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" s="3" t="s">
+      <c r="C43" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G43" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="2">
+      <c r="G43" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
         <v>43</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G44" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="2">
+      <c r="A45" s="3">
         <v>44</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="G45" s="3" t="s">
         <v>98</v>
       </c>
     </row>
+    <row r="46" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>45</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:G46" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="FAIL"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="pass, fail, not executed" sqref="G1" xr:uid="{DFD7D8B4-E7BA-4987-A6DA-68E0D8C1A596}"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G94" xr:uid="{0571C8B8-D6E1-45CF-B917-FC2C17151563}">

</xml_diff>